<commit_message>
Mejoramos a 0.55 aprox métricas STRICT
</commit_message>
<xml_diff>
--- a/Resultados_Anonimizador_Hibrido_v3.xlsx
+++ b/Resultados_Anonimizador_Hibrido_v3.xlsx
@@ -1427,7 +1427,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.5789473684210527</v>
       </c>
     </row>
     <row r="6">
@@ -1487,7 +1487,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4146341463414634</v>
+        <v>0.5365853658536586</v>
       </c>
     </row>
     <row r="7">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4594594594594595</v>
+        <v>0.5569620253164557</v>
       </c>
     </row>
     <row r="8">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.7575757575757576</v>
+        <v>0.7368421052631579</v>
       </c>
     </row>
     <row r="12">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6097560975609756</v>
+        <v>0.6829268292682927</v>
       </c>
     </row>
     <row r="13">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.6756756756756757</v>
+        <v>0.7088607594936709</v>
       </c>
     </row>
   </sheetData>
@@ -5323,7 +5323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5547,10 +5547,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">34 600 123 123 </t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -5634,115 +5634,115 @@
         <v>4</v>
       </c>
       <c r="B11" t="n">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="C11" t="n">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>0099123</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0.9988105893135071</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="n">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="C12" t="n">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>0.9988105893135071</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C13" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>0.9562344551086426</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="n">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="C14" t="n">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0.9984539151191711</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -5750,86 +5750,86 @@
         <v>6</v>
       </c>
       <c r="B15" t="n">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0.9989408850669861</v>
+        <v>0.9562344551086426</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C16" t="n">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Luis Herrera</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0.9989856481552124</v>
+        <v>0.9984539151191711</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C17" t="n">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>0.9989408850669861</v>
       </c>
     </row>
     <row r="18">
@@ -5837,82 +5837,82 @@
         <v>7</v>
       </c>
       <c r="B18" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="C18" t="n">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>Luis Herrera</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>0.9989856481552124</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C19" t="n">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0.6440917253494263</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="C20" t="n">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>52 años</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -5924,28 +5924,28 @@
         <v>8</v>
       </c>
       <c r="B21" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>Roberto Sánchez</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0.9968382716178894</v>
+        <v>0.6440917253494263</v>
       </c>
     </row>
     <row r="22">
@@ -5953,198 +5953,198 @@
         <v>8</v>
       </c>
       <c r="B22" t="n">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>52 años</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0.9989843964576721</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C23" t="n">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220, 28027 Madrid</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0.9992307424545288</v>
+        <v>0.9968382716178894</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B24" t="n">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C24" t="n">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>0.9989843964576721</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B25" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C25" t="n">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Elena Torres</t>
+          <t>C/ Alcalá 220, 28027 Madrid</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0.9993487596511841</v>
+        <v>0.9992307424545288</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B26" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C26" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>145-88</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>0.5947571992874146</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B27" t="n">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C27" t="n">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>0.9988794326782227</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B28" t="n">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C28" t="n">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t xml:space="preserve">34 722 334 112 </t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -6153,175 +6153,320 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B29" t="n">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="C29" t="n">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>Elena Torres</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>0.9993487596511841</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B30" t="n">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C30" t="n">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0.9981183409690857</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B31" t="n">
+        <v>24</v>
+      </c>
+      <c r="C31" t="n">
         <v>34</v>
       </c>
-      <c r="C31" t="n">
-        <v>44</v>
-      </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0.9990630149841309</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C32" t="n">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>hospital</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>0.9917227625846863</v>
+        <v>0.9988794326782227</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" t="n">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C33" t="n">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>0.6910634636878967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
+        <v>14</v>
+      </c>
+      <c r="B34" t="n">
+        <v>76</v>
+      </c>
+      <c r="C34" t="n">
+        <v>98</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>roberto.san@outlook.es</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>15</v>
+      </c>
+      <c r="B35" t="n">
+        <v>12</v>
+      </c>
+      <c r="C35" t="n">
+        <v>22</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>NOMBRE_PACIENTE</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>NOMBRE_PACIENTE</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Marta Ruiz</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>0.9981183409690857</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>15</v>
+      </c>
+      <c r="B36" t="n">
+        <v>34</v>
+      </c>
+      <c r="C36" t="n">
+        <v>44</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>08/06/1990</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>0.9990630149841309</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
         <v>16</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B37" t="n">
+        <v>3</v>
+      </c>
+      <c r="C37" t="n">
+        <v>11</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>hospital</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0.9917227625846863</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>16</v>
+      </c>
+      <c r="B38" t="n">
+        <v>12</v>
+      </c>
+      <c r="C38" t="n">
+        <v>31</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Centro Médico Norte</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0.6910634636878967</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>16</v>
+      </c>
+      <c r="B39" t="n">
         <v>53</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C39" t="n">
         <v>63</v>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="G34" t="n">
+      <c r="G39" t="n">
         <v>0.9989587664604187</v>
       </c>
     </row>
@@ -6398,36 +6543,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fecha de alta</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -6448,36 +6593,36 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>fECHA</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -6498,36 +6643,36 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -6548,36 +6693,36 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -6598,36 +6743,36 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -6648,36 +6793,36 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -6698,36 +6843,36 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -6748,36 +6893,36 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -6798,36 +6943,36 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -6848,36 +6993,36 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Emali</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -6998,36 +7143,36 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -7048,36 +7193,36 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Emali</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -7098,36 +7243,36 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Hospitl</t>
+          <t>Fecha de alta</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -7148,11 +7293,11 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>fECHA</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -7162,7 +7307,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -7177,7 +7322,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -7198,36 +7343,36 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -7267,19 +7412,27 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+          <t>TELEFONO</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>TELEFONO</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>+34 600 123 123</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -7290,38 +7443,46 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>Hospitl</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Centro Médico Norte</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -7332,38 +7493,46 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fecha Ingreso</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>10.0.0.55</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -7374,38 +7543,46 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Dr. Luis Herrera</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>roberto.san@outlook.es</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -7416,38 +7593,46 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>NªSeguro Médico</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+          <t>INSURANCE_ID</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>INSURANCE_ID</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>INS-145-88</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -7458,21 +7643,21 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Código Postal</t>
+          <t>NªHistoría clínica</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>28013</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -7504,17 +7689,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Nombre de Paciente</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -7542,21 +7727,21 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -7584,21 +7769,21 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ID DISPOSITIVO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -7626,21 +7811,21 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Nombre de Paciente</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220</t>
+          <t>Roberto Sánchez</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -7668,21 +7853,21 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NªHistoría clínica</t>
+          <t>Código Postal</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>28013</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -7710,7 +7895,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -7724,7 +7909,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -7752,21 +7937,21 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>Pasaporte</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>PASAPORTE</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -7794,21 +7979,21 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>NªSeguro Médico</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>Dr. Luis Herrera</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -7836,7 +8021,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -7850,7 +8035,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -7878,21 +8063,21 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>Dra. Elena Torres</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -7920,21 +8105,21 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Pasaporte</t>
+          <t>Fecha de ingreso</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PASAPORTE</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -7962,21 +8147,21 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Dra. Elena Torres</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -8008,17 +8193,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -8046,21 +8231,21 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Fecha de ingreso</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -8088,21 +8273,21 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Nº Historia Clínica</t>
+          <t>Fecha Ingreso</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>HC-0099123</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -8172,21 +8357,21 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Fecha Nacimiento</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ID DISPOSITIVO</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>1990-08-06 00:00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -8214,21 +8399,21 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Fecha Nacimiento</t>
+          <t>Nº Historia Clínica</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1990-08-06 00:00:00</t>
+          <t>HC-0099123</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -8256,7 +8441,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -8277,7 +8462,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -8298,7 +8483,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -8309,17 +8494,17 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>hospital</t>
+          <t>Roberto Sánchez</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -8340,7 +8525,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -8351,17 +8536,17 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Luis Herrera</t>
+          <t>C/ Mayor 15, 3B, 28013 Madrid</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -8382,7 +8567,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -8393,17 +8578,17 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t xml:space="preserve">34 600 123 123 </t>
+          <t>45 años</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -8424,7 +8609,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -8435,17 +8620,17 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>C/ Alcalá 220, 28027 Madrid</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -8466,7 +8651,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -8477,17 +8662,17 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>45 años</t>
+          <t>Elena Torres</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -8508,7 +8693,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -8519,17 +8704,17 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220, 28027 Madrid</t>
+          <t>0099123</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -8550,7 +8735,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -8561,17 +8746,17 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>52 años</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -8592,7 +8777,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -8603,17 +8788,17 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>145-88</t>
+          <t>Luis Herrera</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -8634,7 +8819,7 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -8645,17 +8830,17 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>hospital</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -8676,7 +8861,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -8687,17 +8872,17 @@
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B, 28013 Madrid</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -8718,7 +8903,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -8729,17 +8914,17 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t xml:space="preserve">34 722 334 112 </t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -8760,7 +8945,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -8771,17 +8956,17 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Elena Torres</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -8802,7 +8987,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -8813,17 +8998,17 @@
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>52 años</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -8844,7 +9029,7 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -8865,7 +9050,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -8886,7 +9071,7 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -8897,17 +9082,17 @@
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -8937,7 +9122,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9502,14 +9687,14 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t xml:space="preserve">34 600 123 123 </t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K10" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -9836,7 +10021,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ID DISPOSITIVO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -9852,21 +10037,33 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+          <t>DEVICE_ID</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>DEVICE_ID</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>DEV-ABC-123</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>69</v>
+      </c>
+      <c r="K16" t="n">
+        <v>80</v>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -10744,7 +10941,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ID DISPOSITIVO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -10760,21 +10957,33 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
+          <t>DEVICE_ID</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>DEVICE_ID</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>DEV-XYZ-99</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>68</v>
+      </c>
+      <c r="K32" t="n">
+        <v>78</v>
+      </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -10922,21 +11131,33 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
+          <t>INSURANCE_ID</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>INSURANCE_ID</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>INS-145-88</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>24</v>
+      </c>
+      <c r="K35" t="n">
+        <v>34</v>
+      </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
@@ -11044,14 +11265,14 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t xml:space="preserve">34 722 334 112 </t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="J37" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K37" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
@@ -11469,7 +11690,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -11482,21 +11703,21 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>0099123</t>
         </is>
       </c>
       <c r="J45" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K45" t="n">
         <v>65</v>
@@ -11519,7 +11740,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -11532,24 +11753,24 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="K46" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -11582,24 +11803,24 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>Roberto Sánchez</t>
         </is>
       </c>
       <c r="J47" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
@@ -11619,7 +11840,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -11632,24 +11853,24 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>145-88</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="J48" t="n">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="K48" t="n">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
@@ -11669,7 +11890,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -11682,24 +11903,24 @@
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="J49" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="K49" t="n">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
@@ -11719,7 +11940,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -11732,36 +11953,136 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
+          <t>NHC</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>NHC</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>MRN-556677</t>
+        </is>
+      </c>
+      <c r="J50" t="n">
+        <v>73</v>
+      </c>
+      <c r="K50" t="n">
+        <v>83</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>✗</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>lenient</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>15</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>08/06/1990</t>
+        </is>
+      </c>
+      <c r="J51" t="n">
+        <v>34</v>
+      </c>
+      <c r="K51" t="n">
+        <v>44</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>✗</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>lenient</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>16</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
           <t>HOSPITAL</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t>HOSPITAL</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
+      <c r="I52" t="inlineStr">
         <is>
           <t>hospital</t>
         </is>
       </c>
-      <c r="J50" t="n">
+      <c r="J52" t="n">
         <v>3</v>
       </c>
-      <c r="K50" t="n">
+      <c r="K52" t="n">
         <v>11</v>
       </c>
-      <c r="L50" t="inlineStr">
+      <c r="L52" t="inlineStr">
         <is>
           <t>✗</t>
         </is>
       </c>
-      <c r="M50" t="inlineStr">
+      <c r="M52" t="inlineStr">
         <is>
           <t>FP</t>
         </is>
       </c>
-      <c r="N50" t="inlineStr">
+      <c r="N52" t="inlineStr">
         <is>
           <t>lenient</t>
         </is>
@@ -11844,7 +12165,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Se contactó al paciente en el teléfono +Phone_XXXy en el correo Mail_XXX.</t>
+          <t>Se contactó al paciente en el teléfono Phone_XXX y en el correo Mail_XXX.</t>
         </is>
       </c>
     </row>
@@ -11859,7 +12180,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>El paciente con DNI ID_XXXXX y Nº de historia clínica HC-0099123 fue dado de alta el &lt;DATE_DISCHARGE&gt;.</t>
+          <t>El paciente con DNI ID_XXXXX y Nº de historia clínica HC-&lt;MRN&gt; fue dado de alta el &lt;DATE_DISCHARGE&gt;.</t>
         </is>
       </c>
     </row>
@@ -11874,7 +12195,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Accedió al portal desde la IP IP_XXX utilizando el dispositivo DEV-ABC-123.</t>
+          <t>Accedió al portal desde la IP IP_XXX utilizando el dispositivo &lt;DEVICE_ID&gt;.</t>
         </is>
       </c>
     </row>
@@ -11951,7 +12272,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>El número de pasaporte XK987654 fue verificado durante la admisión.</t>
+          <t>El número de pasaporte &lt;DEVICE_ID&gt; fue verificado durante la admisión.</t>
         </is>
       </c>
     </row>
@@ -11966,7 +12287,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>El paciente accedió desde la IP IP_XXX utilizando el dispositivo DEV-XYZ-99.</t>
+          <t>El paciente accedió desde la IP IP_XXX utilizando el dispositivo &lt;DEVICE_ID&gt;.</t>
         </is>
       </c>
     </row>
@@ -11981,7 +12302,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>La profesional sanitaria Dra. &lt;PROVIDER_NAME&gt; actualizó la historia clínica MRN-556677.</t>
+          <t>La profesional sanitaria Dra. &lt;PROVIDER_NAME&gt; actualizó la historia clínica &lt;MRN&gt;.</t>
         </is>
       </c>
     </row>
@@ -11996,7 +12317,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>El seguro médico con ID INS-&lt;PATIENT_NAME&gt; fue validado el &lt;DATE&gt;.</t>
+          <t>El seguro médico con ID &lt;INSURANCE_ID&gt; fue validado el &lt;DATE&gt;.</t>
         </is>
       </c>
     </row>
@@ -12011,7 +12332,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Se notificó al paciente en el teléfono +Phone_XXXy mediante el correo Mail_XXX</t>
+          <t>Se notificó al paciente en el teléfono Phone_XXX y mediante el correo Mail_XXX</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mejoras strict y lenient
</commit_message>
<xml_diff>
--- a/Resultados_Anonimizador_Hibrido_v3.xlsx
+++ b/Resultados_Anonimizador_Hibrido_v3.xlsx
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5789473684210527</v>
+        <v>0.6285714285714286</v>
       </c>
     </row>
     <row r="6">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5569620253164557</v>
+        <v>0.5789473684210527</v>
       </c>
     </row>
     <row r="8">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.7368421052631579</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="12">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.7088607594936709</v>
+        <v>0.736842105263158</v>
       </c>
     </row>
   </sheetData>
@@ -5323,7 +5323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5634,57 +5634,57 @@
         <v>4</v>
       </c>
       <c r="B11" t="n">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="C11" t="n">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0099123</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0.9988105893135071</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="n">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="C12" t="n">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0.9988105893135071</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -5692,24 +5692,24 @@
         <v>5</v>
       </c>
       <c r="B13" t="n">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="C13" t="n">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -5718,31 +5718,31 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" t="n">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0.9562344551086426</v>
       </c>
     </row>
     <row r="15">
@@ -5750,28 +5750,28 @@
         <v>6</v>
       </c>
       <c r="B15" t="n">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0.9562344551086426</v>
+        <v>0.9984539151191711</v>
       </c>
     </row>
     <row r="16">
@@ -5779,57 +5779,57 @@
         <v>6</v>
       </c>
       <c r="B16" t="n">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C16" t="n">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0.9984539151191711</v>
+        <v>0.9989408850669861</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" t="n">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C17" t="n">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>Luis Herrera</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0.9989408850669861</v>
+        <v>0.9989856481552124</v>
       </c>
     </row>
     <row r="18">
@@ -5837,28 +5837,28 @@
         <v>7</v>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Luis Herrera</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0.9989856481552124</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -5866,24 +5866,24 @@
         <v>7</v>
       </c>
       <c r="B19" t="n">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="C19" t="n">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -5892,27 +5892,27 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C20" t="n">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>52 años</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -5924,28 +5924,28 @@
         <v>8</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0.6440917253494263</v>
+        <v>0.9968382716178894</v>
       </c>
     </row>
     <row r="22">
@@ -5953,126 +5953,126 @@
         <v>8</v>
       </c>
       <c r="B22" t="n">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C22" t="n">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>52 años</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0.9989843964576721</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>C/ Alcalá 220, 28027 Madrid</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0.9968382716178894</v>
+        <v>0.9992307424545288</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B24" t="n">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>0.9989843964576721</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B25" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C25" t="n">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220, 28027 Madrid</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0.9992307424545288</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B26" t="n">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C26" t="n">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -6086,7 +6086,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -6095,56 +6095,56 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>Elena Torres</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>0.9993487596511841</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B28" t="n">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="C28" t="n">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -6153,56 +6153,56 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B29" t="n">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C29" t="n">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Elena Torres</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>0.9993487596511841</v>
+        <v>0.9988794326782227</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B30" t="n">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="C30" t="n">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -6211,27 +6211,27 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B31" t="n">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="C31" t="n">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -6240,129 +6240,129 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B32" t="n">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="C32" t="n">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>0.9988794326782227</v>
+        <v>0.9981183409690857</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B33" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C33" t="n">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0.9990630149841309</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B34" t="n">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>hospital</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>0.9917227625846863</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B35" t="n">
         <v>12</v>
       </c>
       <c r="C35" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0.9981183409690857</v>
+        <v>0.6910634636878967</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B36" t="n">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C36" t="n">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -6376,97 +6376,10 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0.9990630149841309</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>16</v>
-      </c>
-      <c r="B37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C37" t="n">
-        <v>11</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>HOSPITAL</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>HOSPITAL</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>hospital</t>
-        </is>
-      </c>
-      <c r="G37" t="n">
-        <v>0.9917227625846863</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>16</v>
-      </c>
-      <c r="B38" t="n">
-        <v>12</v>
-      </c>
-      <c r="C38" t="n">
-        <v>31</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>HOSPITAL</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>HOSPITAL</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Centro Médico Norte</t>
-        </is>
-      </c>
-      <c r="G38" t="n">
-        <v>0.6910634636878967</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>16</v>
-      </c>
-      <c r="B39" t="n">
-        <v>53</v>
-      </c>
-      <c r="C39" t="n">
-        <v>63</v>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>FECHA</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>FECHA</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>05/05/2025</t>
-        </is>
-      </c>
-      <c r="G39" t="n">
         <v>0.9989587664604187</v>
       </c>
     </row>
@@ -6481,7 +6394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6543,36 +6456,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -6593,36 +6506,36 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -6643,36 +6556,36 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -6693,36 +6606,36 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -6743,36 +6656,36 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Fecha de alta</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -6793,36 +6706,36 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Hospitl</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -6843,36 +6756,36 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -6893,36 +6806,36 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -6943,36 +6856,36 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -6993,36 +6906,36 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Emali</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -7093,36 +7006,36 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DNI/NIF</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -7143,36 +7056,36 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Emali</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -7193,36 +7106,36 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>DNI/NIF</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -7243,36 +7156,36 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Fecha de alta</t>
+          <t>fECHA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -7293,36 +7206,36 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>fECHA</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -7343,36 +7256,36 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -7393,36 +7306,36 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>NªSeguro Médico</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -7443,11 +7356,11 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Hospitl</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -7457,7 +7370,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -7472,7 +7385,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -7493,36 +7406,36 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -7543,36 +7456,36 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -7593,36 +7506,36 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NªSeguro Médico</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -7643,21 +7556,21 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>NªHistoría clínica</t>
+          <t>Fecha Nacimiento</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>1990-08-06 00:00:00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -7685,21 +7598,21 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Nº Historia Clínica</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>HC-0099123</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -7727,21 +7640,21 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>Dra. Elena Torres</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -7769,11 +7682,11 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>Código Postal</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -7783,7 +7696,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>28013</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -7811,21 +7724,21 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Nombre de Paciente</t>
+          <t>Fecha de ingreso</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -7853,21 +7766,21 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Código Postal</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>28013</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -7895,21 +7808,21 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Fecha de ingreso</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -7937,21 +7850,21 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Pasaporte</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>PASAPORTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>Dr. Luis Herrera</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -7979,21 +7892,21 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Fecha Ingreso</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Dr. Luis Herrera</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -8021,21 +7934,21 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Fecha de ingreso</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -8063,21 +7976,21 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Dra. Elena Torres</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -8105,21 +8018,21 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fecha de ingreso</t>
+          <t>Código Postal</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>28027</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -8151,17 +8064,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -8189,11 +8102,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -8203,7 +8116,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -8231,21 +8144,21 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Pasaporte</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>PASAPORTE</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -8277,17 +8190,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fecha Ingreso</t>
+          <t>Nombre de Paciente</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>Roberto Sánchez</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -8315,21 +8228,21 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Código Postal</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>28027</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -8357,21 +8270,21 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Fecha Nacimiento</t>
+          <t>NªHistoría clínica</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1990-08-06 00:00:00</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -8399,21 +8312,21 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Nº Historia Clínica</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>HC-0099123</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -8441,7 +8354,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -8452,17 +8365,17 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -8483,7 +8396,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -8494,17 +8407,17 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>C/ Mayor 15, 3B, 28013 Madrid</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -8525,7 +8438,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -8536,17 +8449,17 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B, 28013 Madrid</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -8567,7 +8480,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -8578,17 +8491,17 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>45 años</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -8609,7 +8522,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -8620,17 +8533,17 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220, 28027 Madrid</t>
+          <t>52 años</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -8651,7 +8564,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -8662,17 +8575,17 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Elena Torres</t>
+          <t>hospital</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -8693,7 +8606,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -8704,17 +8617,17 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>0099123</t>
+          <t>Elena Torres</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -8735,7 +8648,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -8746,17 +8659,17 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -8777,7 +8690,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -8788,17 +8701,17 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Luis Herrera</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -8819,7 +8732,7 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -8830,17 +8743,17 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>hospital</t>
+          <t>Luis Herrera</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -8861,7 +8774,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -8882,7 +8795,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -8903,7 +8816,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -8914,17 +8827,17 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>C/ Alcalá 220, 28027 Madrid</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -8945,7 +8858,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -8956,17 +8869,17 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>45 años</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -8980,132 +8893,6 @@
         </is>
       </c>
       <c r="J55" t="inlineStr">
-        <is>
-          <t>strict</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>8</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>EDAD</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>EDAD</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>52 años</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>strict</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>8</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>FECHA</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>FECHA</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>22/11/2025</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>strict</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>10</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>DEVICE_ID</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>DEVICE_ID</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>XK987654</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
         <is>
           <t>strict</t>
         </is>
@@ -9122,7 +8909,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11690,7 +11477,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -11703,21 +11490,21 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>0099123</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="J45" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K45" t="n">
         <v>65</v>
@@ -11740,7 +11527,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -11763,14 +11550,14 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="J46" t="n">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="K46" t="n">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -11790,7 +11577,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -11803,24 +11590,24 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K47" t="n">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
@@ -11840,7 +11627,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -11863,14 +11650,14 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="J48" t="n">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="K48" t="n">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
@@ -11890,7 +11677,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -11903,24 +11690,24 @@
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>hospital</t>
         </is>
       </c>
       <c r="J49" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="K49" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
@@ -11933,156 +11720,6 @@
         </is>
       </c>
       <c r="N49" t="inlineStr">
-        <is>
-          <t>lenient</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>12</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>NHC</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>NHC</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>MRN-556677</t>
-        </is>
-      </c>
-      <c r="J50" t="n">
-        <v>73</v>
-      </c>
-      <c r="K50" t="n">
-        <v>83</v>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>lenient</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>15</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>FECHA</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>FECHA</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>08/06/1990</t>
-        </is>
-      </c>
-      <c r="J51" t="n">
-        <v>34</v>
-      </c>
-      <c r="K51" t="n">
-        <v>44</v>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>lenient</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>16</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>HOSPITAL</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>HOSPITAL</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>hospital</t>
-        </is>
-      </c>
-      <c r="J52" t="n">
-        <v>3</v>
-      </c>
-      <c r="K52" t="n">
-        <v>11</v>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
         <is>
           <t>lenient</t>
         </is>
@@ -12180,7 +11817,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>El paciente con DNI ID_XXXXX y Nº de historia clínica HC-&lt;MRN&gt; fue dado de alta el &lt;DATE_DISCHARGE&gt;.</t>
+          <t>El paciente con DNI ID_XXXXX y Nº de historia clínica HC-0099123 fue dado de alta el &lt;DATE_DISCHARGE&gt;.</t>
         </is>
       </c>
     </row>
@@ -12242,7 +11879,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>&lt;PROVIDER_NAME&gt;, de Age_XX, ingresó en la &lt;HOSPITAL_NAME&gt; el &lt;DATE&gt;.</t>
+          <t>Roberto Sánchez, de Age_XX, ingresó en la &lt;HOSPITAL_NAME&gt; el &lt;DATE&gt;.</t>
         </is>
       </c>
     </row>
@@ -12302,7 +11939,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>La profesional sanitaria Dra. &lt;PROVIDER_NAME&gt; actualizó la historia clínica &lt;MRN&gt;.</t>
+          <t>La profesional sanitaria Dra. &lt;PROVIDER_NAME&gt; actualizó la historia clínica MRN-556677.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Todas las métricas +0.7
</commit_message>
<xml_diff>
--- a/Resultados_Anonimizador_Hibrido_v3.xlsx
+++ b/Resultados_Anonimizador_Hibrido_v3.xlsx
@@ -1427,7 +1427,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.6486486486486487</v>
+        <v>0.7317073170731707</v>
       </c>
     </row>
     <row r="6">
@@ -1487,7 +1487,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5853658536585366</v>
+        <v>0.7317073170731707</v>
       </c>
     </row>
     <row r="7">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.6153846153846153</v>
+        <v>0.7317073170731707</v>
       </c>
     </row>
     <row r="8">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.7567567567567568</v>
+        <v>0.7804878048780488</v>
       </c>
     </row>
     <row r="12">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6829268292682927</v>
+        <v>0.7804878048780488</v>
       </c>
     </row>
     <row r="13">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.7179487179487181</v>
+        <v>0.7804878048780488</v>
       </c>
     </row>
   </sheetData>
@@ -5323,7 +5323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5521,7 +5521,7 @@
         <v>45</v>
       </c>
       <c r="C7" t="n">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B, 28013 Madrid</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -5544,85 +5544,85 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="n">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C8" t="n">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>28013</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0.9976170063018799</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" t="n">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0.9991710186004639</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C10" t="n">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -5631,27 +5631,27 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" t="n">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C11" t="n">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0099123</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -5663,53 +5663,53 @@
         <v>4</v>
       </c>
       <c r="B12" t="n">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0.9988105893135071</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="n">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C13" t="n">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>0099123</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -5718,89 +5718,89 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="n">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C14" t="n">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0.9988105893135071</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C15" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0.9562344551086426</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="n">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="C16" t="n">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0.9984539151191711</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -5808,86 +5808,86 @@
         <v>6</v>
       </c>
       <c r="B17" t="n">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0.9989408850669861</v>
+        <v>0.9562344551086426</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Luis Herrera</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0.9989856481552124</v>
+        <v>0.9984539151191711</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C19" t="n">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>1</v>
+        <v>0.9989408850669861</v>
       </c>
     </row>
     <row r="20">
@@ -5895,53 +5895,53 @@
         <v>7</v>
       </c>
       <c r="B20" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>Luis Herrera</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>0.9989856481552124</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C21" t="n">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -5950,31 +5950,31 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C22" t="n">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0.9968382716178894</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -5982,198 +5982,198 @@
         <v>8</v>
       </c>
       <c r="B23" t="n">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C23" t="n">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>52</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0.9989843964576721</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C24" t="n">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220, 28027 Madrid</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>0.9992307424545288</v>
+        <v>0.9968382716178894</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B25" t="n">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C25" t="n">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>0.9989843964576721</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C26" t="n">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>0.9992307424545288</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B27" t="n">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C27" t="n">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>28027</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>0.9981446266174316</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B28" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C28" t="n">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Elena Torres</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>0.9993487596511841</v>
+        <v>0.9991428852081299</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" t="n">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="C29" t="n">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -6182,27 +6182,27 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C30" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -6211,85 +6211,85 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B31" t="n">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C31" t="n">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0.9988794326782227</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C32" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>Elena Torres</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>0.9993487596511841</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B33" t="n">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C33" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -6298,42 +6298,42 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C34" t="n">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>0.9981183409690857</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B35" t="n">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C35" t="n">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -6347,97 +6347,213 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0.9990630149841309</v>
+        <v>0.9988794326782227</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C36" t="n">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>hospital</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0.9917227625846863</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B37" t="n">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="C37" t="n">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>0.6910634636878967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
+        <v>15</v>
+      </c>
+      <c r="B38" t="n">
+        <v>12</v>
+      </c>
+      <c r="C38" t="n">
+        <v>22</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>NOMBRE_PACIENTE</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>NOMBRE_PACIENTE</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Marta Ruiz</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0.9981183409690857</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>15</v>
+      </c>
+      <c r="B39" t="n">
+        <v>34</v>
+      </c>
+      <c r="C39" t="n">
+        <v>44</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>08/06/1990</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0.9990630149841309</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
         <v>16</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B40" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" t="n">
+        <v>11</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>hospital</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>0.9917227625846863</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>16</v>
+      </c>
+      <c r="B41" t="n">
+        <v>12</v>
+      </c>
+      <c r="C41" t="n">
+        <v>31</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Centro Médico Norte</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>0.6910634636878967</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>16</v>
+      </c>
+      <c r="B42" t="n">
         <v>53</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C42" t="n">
         <v>63</v>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="G38" t="n">
+      <c r="G42" t="n">
         <v>0.9989587664604187</v>
       </c>
     </row>
@@ -6452,7 +6568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6514,36 +6630,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -6564,36 +6680,36 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>45</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -6614,36 +6730,36 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -6664,36 +6780,36 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -6714,36 +6830,36 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NªSeguro Médico</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -6768,32 +6884,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -6814,36 +6930,36 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -6864,36 +6980,36 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Hospitl</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -6918,32 +7034,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fecha de alta</t>
+          <t>DNI/NIF</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -6964,36 +7080,36 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hospitl</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -7018,32 +7134,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Emali</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -7064,36 +7180,36 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Fecha de alta</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -7114,36 +7230,36 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -7164,36 +7280,36 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -7214,36 +7330,36 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>NªSeguro Médico</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -7264,36 +7380,36 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -7314,36 +7430,36 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -7364,36 +7480,36 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DNI/NIF</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -7414,36 +7530,36 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -7464,36 +7580,36 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>fECHA</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -7514,36 +7630,36 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -7564,36 +7680,36 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -7614,36 +7730,36 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Emali</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -7664,36 +7780,36 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>fECHA</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -7714,38 +7830,46 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Código Postal</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>28013</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Hospital La Paz</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -7756,38 +7880,46 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fecha de ingreso</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>juan.perez@gmail.com</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -7798,38 +7930,46 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Dra. Elena Torres</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
+          <t>NOMBRE_PACIENTE</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>NOMBRE_PACIENTE</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ana Martínez</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -7840,38 +7980,46 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Código Postal</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>28027</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>HOSPITAL</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Hospital Virgen del Mar</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -7882,38 +8030,46 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Fecha de ingreso</t>
+          <t>Código Postal</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>28027</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>28027</t>
+        </is>
+      </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -7924,11 +8080,11 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Código Postal</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -7938,24 +8094,32 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220</t>
+          <t>28013</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>28013</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -7966,11 +8130,11 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>NªHistoría clínica</t>
+          <t>Nº Historia Clínica</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -7980,7 +8144,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>HC-0099123</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -8008,21 +8172,21 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Fecha Ingreso</t>
+          <t>Fecha Nacimiento</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -8092,21 +8256,21 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fecha Nacimiento</t>
+          <t>Fecha de ingreso</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -8134,21 +8298,21 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Nº Historia Clínica</t>
+          <t>Pasaporte</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>PASAPORTE</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>HC-0099123</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -8176,21 +8340,21 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Pasaporte</t>
+          <t>Fecha Ingreso</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PASAPORTE</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -8218,21 +8382,21 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>Dr. Luis Herrera</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -8260,21 +8424,21 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>NªHistoría clínica</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -8302,21 +8466,21 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -8344,21 +8508,21 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Dra. Elena Torres</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -8386,21 +8550,21 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Fecha de ingreso</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Dr. Luis Herrera</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -8439,17 +8603,17 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>Elena Torres</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -8470,7 +8634,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -8481,17 +8645,17 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>hospital</t>
+          <t>0099123</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -8512,7 +8676,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -8523,17 +8687,17 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -8554,7 +8718,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -8575,7 +8739,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -8607,17 +8771,17 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -8680,7 +8844,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -8691,17 +8855,17 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220, 28027 Madrid</t>
+          <t>hospital</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -8722,7 +8886,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -8733,17 +8897,17 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -8775,17 +8939,17 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -8817,17 +8981,17 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Elena Torres</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -8848,7 +9012,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -8869,7 +9033,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -8883,90 +9047,6 @@
         </is>
       </c>
       <c r="J53" t="inlineStr">
-        <is>
-          <t>strict</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>2</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>DIRECCION</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>DIRECCION</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>C/ Mayor 15, 3B, 28013 Madrid</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>strict</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>4</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>NHC</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>NHC</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>0099123</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
         <is>
           <t>strict</t>
         </is>
@@ -9386,14 +9466,14 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B, 28013 Madrid</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="J7" t="n">
         <v>45</v>
       </c>
       <c r="K7" t="n">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -9438,21 +9518,33 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>28013</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>62</v>
+      </c>
+      <c r="K8" t="n">
+        <v>67</v>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -9488,21 +9580,33 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Madrid</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>68</v>
+      </c>
+      <c r="K9" t="n">
+        <v>74</v>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -10554,14 +10658,14 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220, 28027 Madrid</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="J27" t="n">
         <v>39</v>
       </c>
       <c r="K27" t="n">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
@@ -10606,21 +10710,33 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>28027</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>54</v>
+      </c>
+      <c r="K28" t="n">
+        <v>59</v>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -10656,21 +10772,33 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Madrid</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>60</v>
+      </c>
+      <c r="K29" t="n">
+        <v>66</v>
+      </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -11961,7 +12089,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>La paciente &lt;PATIENT_NAME&gt;, de Age_XX años, vive en &lt;ADDRESS&gt;.</t>
+          <t>La paciente &lt;PATIENT_NAME&gt;, de Age_XX años, vive en &lt;ADDRESS&gt;, &lt;ADDRESS&gt; &lt;ADDRESS&gt;.</t>
         </is>
       </c>
     </row>
@@ -12068,7 +12196,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Se registró la dirección del paciente: &lt;ADDRESS&gt;.</t>
+          <t>Se registró la dirección del paciente: &lt;ADDRESS&gt;, &lt;ADDRESS&gt; &lt;ADDRESS&gt;.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
formato pasaporte arreglado: Métricas: 0.85
</commit_message>
<xml_diff>
--- a/Resultados_Anonimizador_Hibrido_v3.xlsx
+++ b/Resultados_Anonimizador_Hibrido_v3.xlsx
@@ -6630,36 +6630,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Código Postal</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>28027</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>28027</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -6680,36 +6680,36 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NªSeguro Médico</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -6730,36 +6730,36 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>NªSeguro Médico</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -6780,36 +6780,36 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DNI/NIF</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -6830,36 +6830,36 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Fecha de ingreso</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Dra. Elena Torres</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Dra. Elena Torres</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -6880,36 +6880,36 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Dr. Luis Herrera</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Dr. Luis Herrera</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -6930,36 +6930,36 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -6980,11 +6980,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -6994,7 +6994,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -7009,7 +7009,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -7030,36 +7030,36 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -7080,36 +7080,36 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>fECHA</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -7130,36 +7130,36 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Fecha de alta</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -7180,36 +7180,36 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -7230,36 +7230,36 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -7280,36 +7280,36 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>DNI/NIF</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -7330,36 +7330,36 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Clínica Santa María</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -7380,36 +7380,36 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Dra. Elena Torres</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Dra. Elena Torres</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -7430,36 +7430,36 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -7480,36 +7480,36 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Código Postal</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>28027</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>28027</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -7530,36 +7530,36 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Emali</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -7580,36 +7580,36 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fecha Nacimiento</t>
+          <t>fECHA</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -7630,36 +7630,36 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Fecha de alta</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -7684,32 +7684,32 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Emali</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>Dr. Luis Herrera</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>Dr. Luis Herrera</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -7730,36 +7730,36 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Hospitl</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -7780,36 +7780,36 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -7830,36 +7830,36 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>Clínica Santa María</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -7880,36 +7880,36 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Fecha Nacimiento</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -7934,32 +7934,32 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Código Postal</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>28013</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>28013</t>
+          <t>45</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -7980,36 +7980,36 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -8030,36 +8030,36 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -8080,7 +8080,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -8094,7 +8094,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -8109,7 +8109,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -8130,36 +8130,36 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Hospitl</t>
+          <t>Fecha Ingreso</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>22/11/2025</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -8180,36 +8180,36 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Fecha Ingreso</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>22/11/2025</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -8230,36 +8230,36 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -8280,36 +8280,36 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -8330,36 +8330,36 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Fecha de ingreso</t>
+          <t>Código Postal</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>28013</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>28013</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -8380,11 +8380,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Nombre de Paciente</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -8394,7 +8394,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>Roberto Sánchez</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -8422,11 +8422,11 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Nº Historia Clínica</t>
+          <t>NªHistoría clínica</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -8436,7 +8436,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>HC-0099123</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -8506,21 +8506,21 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Nombre de Paciente</t>
+          <t>Nº Historia Clínica</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>HC-0099123</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -8548,21 +8548,21 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>NªHistoría clínica</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -8632,7 +8632,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -8643,17 +8643,17 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -8674,7 +8674,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -8685,17 +8685,17 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>HC-0099123</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -8716,7 +8716,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -8727,17 +8727,17 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>hospital</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -8758,7 +8758,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -8769,17 +8769,17 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>HC-0099123</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -8800,7 +8800,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -8811,17 +8811,17 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -8842,7 +8842,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -8853,17 +8853,17 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>hospital</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">

</xml_diff>

<commit_message>
Terminado por ahora: 0.92
</commit_message>
<xml_diff>
--- a/Resultados_Anonimizador_Hibrido_v3.xlsx
+++ b/Resultados_Anonimizador_Hibrido_v3.xlsx
@@ -1427,7 +1427,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9024390243902439</v>
+        <v>0.926829268292683</v>
       </c>
     </row>
     <row r="6">
@@ -1487,7 +1487,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9024390243902439</v>
+        <v>0.926829268292683</v>
       </c>
     </row>
     <row r="7">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9024390243902439</v>
+        <v>0.926829268292683</v>
       </c>
     </row>
     <row r="8">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9024390243902439</v>
+        <v>0.926829268292683</v>
       </c>
     </row>
     <row r="12">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9024390243902439</v>
+        <v>0.926829268292683</v>
       </c>
     </row>
     <row r="13">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.9024390243902439</v>
+        <v>0.926829268292683</v>
       </c>
     </row>
   </sheetData>
@@ -5380,12 +5380,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -6568,7 +6568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6634,7 +6634,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>Código Postal</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -6644,7 +6644,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>28027</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -6659,7 +6659,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>28027</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -6680,36 +6680,36 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>DEV-XYZ-99</t>
+          <t>C/ Mayor 15, 3B</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -6730,7 +6730,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -6759,7 +6759,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Hospital Virgen del Mar</t>
+          <t>Hospital La Paz</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -6780,36 +6780,36 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>fECHA</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>03/03/2026</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -6830,36 +6830,36 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ciudad</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Marta Ruiz</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -6880,36 +6880,36 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>10.0.0.55</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -6930,36 +6930,36 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Hospitl</t>
+          <t>Fecha de alta</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_ALTA</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Centro Médico Norte</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -6980,36 +6980,36 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Hospitl</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10.0.0.55</t>
+          <t>Centro Médico Norte</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -7030,36 +7030,36 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DNI/NIF</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>DNI_NIF</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>12345678A</t>
+          <t>juan.perez@gmail.com</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -7080,36 +7080,36 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>+34 722 334 112</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -7180,36 +7180,36 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ID Dispositivo</t>
+          <t>fECHA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>DEVICE_ID</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>DEV-ABC-123</t>
+          <t>03/03/2026</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -7230,36 +7230,36 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>roberto.san@outlook.es</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -7280,36 +7280,36 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nº Historia Clínica</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>HC-0099123</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>HC-0099123</t>
+          <t>Hospital Virgen del Mar</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -7330,36 +7330,36 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Dr. Luis Herrera</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Dr. Luis Herrera</t>
+          <t>C/ Alcalá 220</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -7380,36 +7380,36 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Pasaporte</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>PASAPORTE</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>PASAPORTE</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>PASAPORTE</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Marta Ruiz</t>
+          <t>XK987654</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -7430,36 +7430,36 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Nombre Profesional</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Dra. Elena Torres</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Dra. Elena Torres</t>
+          <t>DEV-ABC-123</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -7480,36 +7480,36 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>912 556 789</t>
+          <t>192.168.1.10</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -7530,36 +7530,36 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>juan.perez@gmail.com</t>
+          <t>912 556 789</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -7580,36 +7580,36 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fecha Nacimiento</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>FECHA_NACIMIENTO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>08/06/1990</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -7630,36 +7630,36 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>Dr. Luis Herrera</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>Dr. Luis Herrera</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -7680,36 +7680,36 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>ID Dispositivo</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>DEVICE_ID</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>+34 722 334 112</t>
+          <t>DEV-XYZ-99</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -7730,36 +7730,36 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pasaporte</t>
+          <t>NªSeguro Médico</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PASAPORTE</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>PASAPORTE</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>PASAPORTE</t>
+          <t>INSURANCE_ID</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>XK987654</t>
+          <t>INS-145-88</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -7780,36 +7780,36 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>C/ Alcalá 220</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -7830,36 +7830,36 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>NªSeguro Médico</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>INSURANCE_ID</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>INS-145-88</t>
+          <t>roberto.san@outlook.es</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -7884,32 +7884,32 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Dirección</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>C/ Mayor 15, 3B</t>
+          <t>María López</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -7930,36 +7930,36 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Fecha de alta</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>FECHA_ALTA</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>45</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -7980,36 +7980,36 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Hospital</t>
+          <t>Fecha Nacimiento</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA_NACIMIENTO</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Hospital La Paz</t>
+          <t>08/06/1990</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -8030,36 +8030,36 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Fecha de ingreso</t>
+          <t>DNI/NIF</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>DNI_NIF</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>12345678A</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -8080,36 +8080,36 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>Fecha de ingreso</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>María López</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -8130,36 +8130,36 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Código Postal</t>
+          <t>Nombre Profesional</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>28013</t>
+          <t>Dra. Elena Torres</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>NOMBRE_PROFESIONAL</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>28013</t>
+          <t>Dra. Elena Torres</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -8180,36 +8180,36 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Emali</t>
+          <t>Nombre Paciente</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>EMAIL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>l.herrera@hospital.com</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -8230,36 +8230,36 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Nº Historia Clínica</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>HC-0099123</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>EDAD</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>HC-0099123</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -8280,7 +8280,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -8294,7 +8294,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>28027</t>
+          <t>28013</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -8309,7 +8309,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>28027</t>
+          <t>28013</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -8330,36 +8330,36 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Teléfono</t>
+          <t>Emali</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>TELEFONO</t>
+          <t>EMAIL</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>+34 600 123 123</t>
+          <t>l.herrera@hospital.com</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -8430,36 +8430,36 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Teléfono</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>192.168.1.10</t>
+          <t>+34 600 123 123</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -8480,38 +8480,46 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fecha de ingreso</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>FECHA_INGRESO</t>
+          <t>EDAD</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+          <t>EDAD</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>EDAD</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -8522,21 +8530,21 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Nombre de Paciente</t>
+          <t>Fecha de ingreso</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>FECHA_INGRESO</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Roberto Sánchez</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -8564,21 +8572,21 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>NªHistoría clínica</t>
+          <t>Nombre de Paciente</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>NOMBRE_PACIENTE</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>Roberto Sánchez</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -8606,21 +8614,21 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Nombre Paciente</t>
+          <t>NªHistoría clínica</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>NOMBRE_PACIENTE</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -8648,7 +8656,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -8659,17 +8667,17 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>hospital</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -8690,7 +8698,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -8701,17 +8709,17 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>HOSPITAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>hospital</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -8767,48 +8775,6 @@
         </is>
       </c>
       <c r="J45" t="inlineStr">
-        <is>
-          <t>strict</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>6</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>FECHA</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>FECHA</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>15/01/2026</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
         <is>
           <t>strict</t>
         </is>
@@ -8825,7 +8791,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8932,21 +8898,33 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+          <t>NOMBRE_PACIENTE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NOMBRE_PACIENTE</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Juan Pérez</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>10</v>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>✗</t>
+          <t>✓</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -11401,7 +11379,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -11414,24 +11392,24 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>NOMBRE_PROFESIONAL</t>
+          <t>FECHA</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="J43" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="K43" t="n">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
@@ -11451,7 +11429,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -11464,24 +11442,24 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>NHC</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>MRN-556677</t>
         </is>
       </c>
       <c r="J44" t="n">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="K44" t="n">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
@@ -11501,7 +11479,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -11514,24 +11492,24 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>NHC</t>
+          <t>HOSPITAL</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>MRN-556677</t>
+          <t>hospital</t>
         </is>
       </c>
       <c r="J45" t="n">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="K45" t="n">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
@@ -11544,56 +11522,6 @@
         </is>
       </c>
       <c r="N45" t="inlineStr">
-        <is>
-          <t>lenient</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>16</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>HOSPITAL</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>HOSPITAL</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>hospital</t>
-        </is>
-      </c>
-      <c r="J46" t="n">
-        <v>3</v>
-      </c>
-      <c r="K46" t="n">
-        <v>11</v>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>FP</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
         <is>
           <t>lenient</t>
         </is>
@@ -11646,7 +11574,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>&lt;PROVIDER_NAME&gt; ingresó en el &lt;HOSPITAL_NAME&gt; el &lt;DATE_ADMISSION&gt; con dolor torácico.</t>
+          <t>&lt;PATIENT_NAME&gt; ingresó en el &lt;HOSPITAL_NAME&gt; el &lt;DATE_ADMISSION&gt; con dolor torácico.</t>
         </is>
       </c>
     </row>

</xml_diff>